<commit_message>
Updated Lecturer email content and highlight risky students in yellow in the excel file, delete Sheet1
</commit_message>
<xml_diff>
--- a/LecturerReports/2401404e_gmail_com.xlsx
+++ b/LecturerReports/2401404e_gmail_com.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liewj\Documents\UiPath\Project\LecturerReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE88031A-A05C-41A1-A00E-20CABDFE963A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057E729A-664F-467E-BCBA-2B5CD250D063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{72ACBDD8-B408-4AFF-AEE1-5B318C8CFB06}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="5" xr2:uid="{72ACBDD8-B408-4AFF-AEE1-5B318C8CFB06}"/>
   </bookViews>
   <sheets>
     <sheet name="1B_Microcontroller" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="1A_Internet of Things Project" sheetId="4" r:id="rId4"/>
     <sheet name="1B_Full Stack Development" sheetId="3" r:id="rId5"/>
     <sheet name="1A_Full Stack Development" sheetId="2" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -384,7 +383,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,13 +391,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -413,8 +424,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A690B1-4FAB-4E03-8D49-52C7EA589267}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -996,22 +1008,22 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>35.71</v>
       </c>
-      <c r="D13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1116,22 +1128,22 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>28.57</v>
       </c>
-      <c r="D19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="D19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1349,22 +1361,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>35.71</v>
       </c>
-      <c r="D2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1749,22 +1761,22 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>28.57</v>
       </c>
-      <c r="D22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2062,22 +2074,22 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>35.71</v>
       </c>
-      <c r="D13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2182,22 +2194,22 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>28.57</v>
       </c>
-      <c r="D19" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="D19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2415,22 +2427,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2595,22 +2607,22 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>64.290000000000006</v>
       </c>
-      <c r="D11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2815,22 +2827,22 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>71.430000000000007</v>
       </c>
-      <c r="D22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3128,22 +3140,22 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>35.71</v>
       </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3248,22 +3260,22 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>28.57</v>
       </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3456,7 +3468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10E6602-FBFC-4957-BF5D-42DFACE35514}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3481,22 +3493,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3661,22 +3673,22 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>64.290000000000006</v>
       </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3881,22 +3893,22 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>71.430000000000007</v>
       </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3943,16 +3955,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0016D71-018D-481D-9074-06D4B4CBF8FB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Made running flowChartMain Obvious
</commit_message>
<xml_diff>
--- a/LecturerReports/2401404e_gmail_com.xlsx
+++ b/LecturerReports/2401404e_gmail_com.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liewj\Documents\UiPath\Project\LecturerReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17049B12-EEA5-4324-8E47-BBE1418FBB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3B4E7C-DF1D-4B4B-9973-22781E094CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{E732133F-E23B-4F7A-B1B1-A8D2CD66C768}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E732133F-E23B-4F7A-B1B1-A8D2CD66C768}"/>
   </bookViews>
   <sheets>
     <sheet name="1A_Microcontroller" sheetId="4" r:id="rId1"/>
@@ -757,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E68C55-CE27-47D5-A4A3-09E948F20C9A}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1823,7 +1823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463EA3ED-933A-4521-8C49-B44FD4F9EA53}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
Final push, dk what i changed
</commit_message>
<xml_diff>
--- a/LecturerReports/2401404e_gmail_com.xlsx
+++ b/LecturerReports/2401404e_gmail_com.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liewj\Documents\UiPath\Project\LecturerReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3B4E7C-DF1D-4B4B-9973-22781E094CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1F6E4D-DC1C-4813-A72B-A57360F0F328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E732133F-E23B-4F7A-B1B1-A8D2CD66C768}"/>
   </bookViews>

</xml_diff>